<commit_message>
issues #26 an #27 added
</commit_message>
<xml_diff>
--- a/presentations/ietf-vs-onf-microwave&ethernetwired-working-doc.xlsx
+++ b/presentations/ietf-vs-onf-microwave&ethernetwired-working-doc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1BB0B95D-323A-432E-ACDA-A2424626B970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CAE71FDD-A7DE-4912-A4AB-814DFA8C8780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4369,7 +4369,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4359" uniqueCount="2260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4364" uniqueCount="2263">
   <si>
     <t>module: ietf-hardware</t>
   </si>
@@ -11187,6 +11187,15 @@
   </si>
   <si>
     <t>association between interface and hardware exists ietf</t>
+  </si>
+  <si>
+    <t>#25</t>
+  </si>
+  <si>
+    <t>#26</t>
+  </si>
+  <si>
+    <t>#27</t>
   </si>
 </sst>
 </file>
@@ -12960,9 +12969,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -13000,7 +13009,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -13106,7 +13115,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -13248,7 +13257,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -28405,10 +28414,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:E628"/>
+  <dimension ref="A1:F628"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="E128" sqref="E128"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -28933,7 +28942,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="76" t="s">
         <v>441</v>
       </c>
@@ -28941,7 +28950,7 @@
         <v>1811</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="42" t="s">
         <v>443</v>
       </c>
@@ -28949,7 +28958,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="42" t="s">
         <v>445</v>
       </c>
@@ -28957,7 +28966,7 @@
         <v>1812</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="77" t="s">
         <v>447</v>
       </c>
@@ -28968,7 +28977,7 @@
         <v>45256</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="42" t="s">
         <v>449</v>
       </c>
@@ -28979,7 +28988,7 @@
         <v>2245</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="78" t="s">
         <v>451</v>
       </c>
@@ -28990,7 +28999,7 @@
         <v>2246</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="77" t="s">
         <v>453</v>
       </c>
@@ -29000,8 +29009,11 @@
       <c r="E71" s="119" t="s">
         <v>2247</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F71" t="s">
+        <v>2260</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="77" t="s">
         <v>455</v>
       </c>
@@ -29011,8 +29023,11 @@
       <c r="E72" s="119" t="s">
         <v>2248</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F72" t="s">
+        <v>2260</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="79" t="s">
         <v>457</v>
       </c>
@@ -29020,8 +29035,11 @@
         <v>1267</v>
       </c>
       <c r="E73" s="119"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F73" t="s">
+        <v>2260</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="79" t="s">
         <v>459</v>
       </c>
@@ -29030,7 +29048,7 @@
       </c>
       <c r="E74" s="119"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="79" t="s">
         <v>461</v>
       </c>
@@ -29039,7 +29057,7 @@
       </c>
       <c r="E75" s="119"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="42" t="s">
         <v>463</v>
       </c>
@@ -29048,7 +29066,7 @@
       </c>
       <c r="E76" s="119"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="80" t="s">
         <v>465</v>
       </c>
@@ -29059,7 +29077,7 @@
         <v>2249</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="80" t="s">
         <v>467</v>
       </c>
@@ -29070,7 +29088,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="42" t="s">
         <v>469</v>
       </c>
@@ -29081,7 +29099,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="82" t="s">
         <v>471</v>
       </c>
@@ -29092,7 +29110,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="82" t="s">
         <v>473</v>
       </c>
@@ -29103,7 +29121,7 @@
         <v>2249</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="42" t="s">
         <v>475</v>
       </c>
@@ -29114,7 +29132,7 @@
         <v>2251</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="85" t="s">
         <v>477</v>
       </c>
@@ -29122,7 +29140,7 @@
         <v>1822</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="85" t="s">
         <v>479</v>
       </c>
@@ -29132,8 +29150,11 @@
       <c r="E84" s="119" t="s">
         <v>2252</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F84" t="s">
+        <v>2261</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="85" t="s">
         <v>481</v>
       </c>
@@ -29144,7 +29165,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="85" t="s">
         <v>483</v>
       </c>
@@ -29155,7 +29176,7 @@
         <v>2253</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="85" t="s">
         <v>485</v>
       </c>
@@ -29166,7 +29187,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="85" t="s">
         <v>487</v>
       </c>
@@ -29177,7 +29198,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="85" t="s">
         <v>489</v>
       </c>
@@ -29187,8 +29208,11 @@
       <c r="E89" s="119" t="s">
         <v>2252</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F89" t="s">
+        <v>2262</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="85" t="s">
         <v>491</v>
       </c>
@@ -29199,7 +29223,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="42" t="s">
         <v>493</v>
       </c>
@@ -29210,7 +29234,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="42" t="s">
         <v>495</v>
       </c>
@@ -29221,7 +29245,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="87" t="s">
         <v>497</v>
       </c>
@@ -29232,7 +29256,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="87" t="s">
         <v>499</v>
       </c>
@@ -29243,7 +29267,7 @@
         <v>2255</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="87" t="s">
         <v>501</v>
       </c>
@@ -29254,7 +29278,7 @@
         <v>2255</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="42" t="s">
         <v>503</v>
       </c>

</xml_diff>